<commit_message>
automate all columns checking
</commit_message>
<xml_diff>
--- a/files/SKU.xlsx
+++ b/files/SKU.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Package category</t>
   </si>
   <si>
-    <t xml:space="preserve">PRTF00001</t>
+    <t xml:space="preserve">PRTS00001</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep Ebi Fry Wok</t>
@@ -107,19 +107,19 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">PRTF00002</t>
+    <t xml:space="preserve">PRTS00002</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Shallow Rebus Work</t>
   </si>
   <si>
-    <t xml:space="preserve">PRTF00003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRTF00004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRTF00005</t>
+    <t xml:space="preserve">PRTS00003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRTS00004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRTS00005</t>
   </si>
 </sst>
 </file>
@@ -264,33 +264,33 @@
   </sheetPr>
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="17.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="10.49"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.6185185185185"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="10.6814814814815"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -684,7 +684,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
+  <conditionalFormatting sqref="A:A">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -733,7 +733,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Add kafka and couchbase check all columns
</commit_message>
<xml_diff>
--- a/files/SKU.xlsx
+++ b/files/SKU.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
   <si>
     <t xml:space="preserve">SKU</t>
   </si>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Package category</t>
   </si>
   <si>
-    <t xml:space="preserve">PRTS00001</t>
+    <t xml:space="preserve">QRTS00001</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep Ebi Fry Wok</t>
@@ -107,19 +107,28 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">PRTS00002</t>
+    <t xml:space="preserve">QRTS00002</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Shallow Rebus Work</t>
   </si>
   <si>
-    <t xml:space="preserve">PRTS00003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRTS00004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRTS00005</t>
+    <t xml:space="preserve">QRTS00003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alcor Deep BEEF Fry Wok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QRTS00004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alcor Shallow KOBE Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QRTS00005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alcor Deep MICIN Fry Wok</t>
   </si>
 </sst>
 </file>
@@ -244,16 +253,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -265,32 +264,32 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.7185185185185"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.9925925925926"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.6185185185185"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6925925925926"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.0111111111111"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -493,7 +492,7 @@
         <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>23</v>
@@ -555,10 +554,10 @@
     </row>
     <row r="5" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -620,10 +619,10 @@
     </row>
     <row r="6" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -684,11 +683,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A:A">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="10">
     <dataValidation allowBlank="true" error="Kode SKU harus diisi dengan kode unik yang terdiri dari 4-20 karakter." errorTitle="SKU" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A1:A6" type="textLength">
       <formula1>4</formula1>

</xml_diff>

<commit_message>
Refactor, comment out the unnecessary
</commit_message>
<xml_diff>
--- a/files/SKU.xlsx
+++ b/files/SKU.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Package category</t>
   </si>
   <si>
-    <t xml:space="preserve">QRTS00001</t>
+    <t xml:space="preserve">KRTD00001</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep Ebi Fry Wok</t>
@@ -107,25 +107,25 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">QRTS00002</t>
+    <t xml:space="preserve">KRTD00002</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Shallow Rebus Work</t>
   </si>
   <si>
-    <t xml:space="preserve">QRTS00003</t>
+    <t xml:space="preserve">KRTD00003</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep BEEF Fry Wok</t>
   </si>
   <si>
-    <t xml:space="preserve">QRTS00004</t>
+    <t xml:space="preserve">KRTD00004</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Shallow KOBE Work</t>
   </si>
   <si>
-    <t xml:space="preserve">QRTS00005</t>
+    <t xml:space="preserve">KRTD00005</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep MICIN Fry Wok</t>
@@ -264,32 +264,29 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6925925925926"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.0925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.0111111111111"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.0814814814815"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.3814814814815"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.2074074074074"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
FiFix timestamp file matching
</commit_message>
<xml_diff>
--- a/files/SKU.xlsx
+++ b/files/SKU.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Package category</t>
   </si>
   <si>
-    <t xml:space="preserve">KRTD00001</t>
+    <t xml:space="preserve">PIPI00001</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep Ebi Fry Wok</t>
@@ -107,25 +107,25 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">KRTD00002</t>
+    <t xml:space="preserve">PIPI00002</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Shallow Rebus Work</t>
   </si>
   <si>
-    <t xml:space="preserve">KRTD00003</t>
+    <t xml:space="preserve">PIPI00003</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep BEEF Fry Wok</t>
   </si>
   <si>
-    <t xml:space="preserve">KRTD00004</t>
+    <t xml:space="preserve">PIPI00004</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Shallow KOBE Work</t>
   </si>
   <si>
-    <t xml:space="preserve">KRTD00005</t>
+    <t xml:space="preserve">PIPI00005</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep MICIN Fry Wok</t>
@@ -264,29 +264,32 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.0814814814815"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.3814814814815"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
move nested loop from robot to python
</commit_message>
<xml_diff>
--- a/files/SKU.xlsx
+++ b/files/SKU.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Package category</t>
   </si>
   <si>
-    <t xml:space="preserve">PIPI00001</t>
+    <t xml:space="preserve">BEAT00001</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep Ebi Fry Wok</t>
@@ -107,25 +107,25 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">PIPI00002</t>
+    <t xml:space="preserve">BEAT00002</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Shallow Rebus Work</t>
   </si>
   <si>
-    <t xml:space="preserve">PIPI00003</t>
+    <t xml:space="preserve">BEAT00003</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep BEEF Fry Wok</t>
   </si>
   <si>
-    <t xml:space="preserve">PIPI00004</t>
+    <t xml:space="preserve">BEAT00004</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Shallow KOBE Work</t>
   </si>
   <si>
-    <t xml:space="preserve">PIPI00005</t>
+    <t xml:space="preserve">BEAT00005</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep MICIN Fry Wok</t>
@@ -269,27 +269,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.8444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.5185185185185"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.362962962963"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
refactor and integrate with web automation framework
</commit_message>
<xml_diff>
--- a/files/SKU.xlsx
+++ b/files/SKU.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Package category</t>
   </si>
   <si>
-    <t xml:space="preserve">BEAT00001</t>
+    <t xml:space="preserve">IMGG00001</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep Ebi Fry Wok</t>
@@ -107,25 +107,25 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">BEAT00002</t>
+    <t xml:space="preserve">IMGG00002</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Shallow Rebus Work</t>
   </si>
   <si>
-    <t xml:space="preserve">BEAT00003</t>
+    <t xml:space="preserve">IMGG00003</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep BEEF Fry Wok</t>
   </si>
   <si>
-    <t xml:space="preserve">BEAT00004</t>
+    <t xml:space="preserve">IMGG00004</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Shallow KOBE Work</t>
   </si>
   <si>
-    <t xml:space="preserve">BEAT00005</t>
+    <t xml:space="preserve">IMGG00005</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep MICIN Fry Wok</t>
@@ -269,27 +269,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.8444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.5185185185185"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.362962962963"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.7259259259259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="24.1074074074074"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.5185185185185"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.9518518518519"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
refactor kafka and couchbase
</commit_message>
<xml_diff>
--- a/files/SKU.xlsx
+++ b/files/SKU.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Package category</t>
   </si>
   <si>
-    <t xml:space="preserve">ABQY00001</t>
+    <t xml:space="preserve">NSQL00001</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep Fry Wok</t>
@@ -107,301 +107,301 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">ABQY00002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00037</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00046</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00047</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00048</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00054</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00068</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00073</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00076</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00078</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00079</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00086</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00087</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00088</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00090</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00092</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00093</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00094</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00095</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00096</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00097</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00098</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABQY00100</t>
+    <t xml:space="preserve">NSQL00002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00092</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSQL00100</t>
   </si>
 </sst>
 </file>
@@ -532,33 +532,33 @@
   </sheetPr>
   <dimension ref="A1:U101"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.8444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.5185185185185"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.362962962963"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.7259259259259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="24.1074074074074"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.5185185185185"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.9518518518519"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Parse kafka message with protobuf
</commit_message>
<xml_diff>
--- a/files/SKU.xlsx
+++ b/files/SKU.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Package category</t>
   </si>
   <si>
-    <t xml:space="preserve">GSQL00001</t>
+    <t xml:space="preserve">TWNT00001</t>
   </si>
   <si>
     <t xml:space="preserve">Alcor Deep Fry Wok</t>
@@ -107,301 +107,301 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">GSQL00002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00037</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00046</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00047</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00048</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00054</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00068</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00073</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00076</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00078</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00079</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00086</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00087</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00088</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00090</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00092</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00093</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00094</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00095</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00096</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00097</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00098</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSQL00100</t>
+    <t xml:space="preserve">TWNT00002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00092</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWNT00100</t>
   </si>
 </sst>
 </file>
@@ -532,33 +532,33 @@
   </sheetPr>
   <dimension ref="A1:U101"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A99" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.5888888888889"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.2814814814815"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="22.9296296296296"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.6481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.1074074074074"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.8703703703704"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="23.9111111111111"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>